<commit_message>
new file:   CHANGELOG_V2.1.txt 	new file:   COMECE_AQUI_WEB.txt 	new file:   README_WEB.txt 	new file:   RESUMO_WEB_V2.1.txt 	new file:   __pycache__/app_streamlit.cpython-312.pyc 	new file:   __pycache__/interface.cpython-312.pyc 	new file:   __pycache__/senior_aut.cpython-312.pyc 	modified:   controle_banco_horas.xlsx 	modified:   dashboard/dashboard_data.json 	new file:   iniciar_web.bat 	modified:   requirements.txt 	renamed:    senior-aut.py -> senior_aut.py
</commit_message>
<xml_diff>
--- a/controle_banco_horas.xlsx
+++ b/controle_banco_horas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,15 +456,20 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Abonas</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Carga Horária</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Banco do Dia</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Saldo Acumulado</t>
         </is>
@@ -489,15 +494,20 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>00:00</t>
         </is>
@@ -526,15 +536,20 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>00:33</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>00:33</t>
         </is>
@@ -563,15 +578,20 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>00:18</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>00:51</t>
         </is>
@@ -600,15 +620,20 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>00:51</t>
         </is>
@@ -637,15 +662,20 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>00:19</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>01:10</t>
         </is>
@@ -674,15 +704,20 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>00:14</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>01:24</t>
         </is>
@@ -711,15 +746,20 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>00:06</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>01:30</t>
         </is>
@@ -748,15 +788,20 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>00:11</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>01:41</t>
         </is>
@@ -785,15 +830,20 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>00:13</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>01:54</t>
         </is>
@@ -822,15 +872,20 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>01:54</t>
         </is>
@@ -859,15 +914,20 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>00:33</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>02:27</t>
         </is>
@@ -896,15 +956,20 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>00:42</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>03:09</t>
         </is>
@@ -929,15 +994,20 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>03:09</t>
         </is>
@@ -966,15 +1036,20 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>00:20</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>03:29</t>
         </is>
@@ -1003,15 +1078,20 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>00:27</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>03:56</t>
         </is>
@@ -1040,15 +1120,20 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>00:04</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>04:00</t>
         </is>
@@ -1077,15 +1162,20 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>-00:10</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>03:50</t>
         </is>
@@ -1114,15 +1204,20 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>00:41</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>04:31</t>
         </is>
@@ -1151,15 +1246,20 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>00:18</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>04:49</t>
         </is>
@@ -1188,15 +1288,20 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>00:18</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>05:07</t>
         </is>
@@ -1225,15 +1330,20 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>00:18</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>05:25</t>
         </is>
@@ -1262,15 +1372,20 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>00:05</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>05:30</t>
         </is>
@@ -1299,15 +1414,20 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>-00:04</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>05:26</t>
         </is>
@@ -1336,15 +1456,20 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>00:24</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>05:50</t>
         </is>
@@ -1373,15 +1498,20 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>00:05</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>05:55</t>
         </is>
@@ -1410,15 +1540,20 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
           <t>00:02</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>05:57</t>
         </is>
@@ -1443,15 +1578,20 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>05:57</t>
         </is>
@@ -1476,15 +1616,20 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
         <is>
           <t>05:57</t>
         </is>
@@ -1513,15 +1658,20 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>00:23</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>06:20</t>
         </is>
@@ -1550,15 +1700,20 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
         <is>
           <t>06:20</t>
         </is>
@@ -1587,15 +1742,20 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
           <t>00:11</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>06:31</t>
         </is>
@@ -1624,15 +1784,20 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
           <t>00:32</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>07:03</t>
         </is>
@@ -1661,15 +1826,20 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
           <t>-00:04</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>06:59</t>
         </is>
@@ -1698,15 +1868,20 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
           <t>-00:03</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t>06:56</t>
         </is>
@@ -1735,15 +1910,20 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
         <is>
           <t>06:56</t>
         </is>
@@ -1772,15 +1952,20 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
           <t>00:20</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>07:16</t>
         </is>
@@ -1809,15 +1994,20 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
           <t>-00:16</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
@@ -1846,15 +2036,20 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
           <t>00:28</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="H39" t="inlineStr">
         <is>
           <t>07:28</t>
         </is>
@@ -1879,15 +2074,20 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
         <is>
           <t>07:28</t>
         </is>
@@ -1916,15 +2116,20 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
           <t>00:20</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t>07:48</t>
         </is>
@@ -1953,15 +2158,20 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
           <t>00:33</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="H42" t="inlineStr">
         <is>
           <t>08:21</t>
         </is>
@@ -1990,15 +2200,20 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
           <t>00:41</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="H43" t="inlineStr">
         <is>
           <t>09:02</t>
         </is>
@@ -2027,15 +2242,20 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
           <t>00:35</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>09:37</t>
         </is>
@@ -2064,15 +2284,20 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
           <t>00:20</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="H45" t="inlineStr">
         <is>
           <t>09:57</t>
         </is>
@@ -2101,15 +2326,20 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
           <t>00:15</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="H46" t="inlineStr">
         <is>
           <t>10:12</t>
         </is>
@@ -2138,15 +2368,20 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
           <t>-00:01</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="H47" t="inlineStr">
         <is>
           <t>10:11</t>
         </is>
@@ -2175,15 +2410,20 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
           <t>00:12</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="H48" t="inlineStr">
         <is>
           <t>10:23</t>
         </is>
@@ -2212,15 +2452,20 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
           <t>-04:00</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="H49" t="inlineStr">
         <is>
           <t>06:23</t>
         </is>
@@ -2245,15 +2490,20 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
         <is>
           <t>06:23</t>
         </is>
@@ -2278,15 +2528,20 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
         <is>
           <t>06:23</t>
         </is>
@@ -2311,15 +2566,20 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
         <is>
           <t>06:23</t>
         </is>
@@ -2344,15 +2604,20 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
         <is>
           <t>06:23</t>
         </is>
@@ -2377,15 +2642,20 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
         <is>
           <t>06:23</t>
         </is>
@@ -2410,15 +2680,20 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
         <is>
           <t>06:23</t>
         </is>
@@ -2443,15 +2718,20 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
         <is>
           <t>06:23</t>
         </is>
@@ -2476,15 +2756,20 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
         <is>
           <t>06:23</t>
         </is>
@@ -2509,15 +2794,20 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
         <is>
           <t>06:23</t>
         </is>
@@ -2542,15 +2832,20 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
         <is>
           <t>06:23</t>
         </is>
@@ -2579,15 +2874,20 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
           <t>00:04</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr">
+      <c r="H60" t="inlineStr">
         <is>
           <t>06:27</t>
         </is>
@@ -2616,15 +2916,20 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
           <t>00:07</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="H61" t="inlineStr">
         <is>
           <t>06:34</t>
         </is>
@@ -2653,15 +2958,20 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
           <t>00:21</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr">
+      <c r="H62" t="inlineStr">
         <is>
           <t>06:55</t>
         </is>
@@ -2690,15 +3000,20 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
         <is>
           <t>06:55</t>
         </is>
@@ -2727,15 +3042,20 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
           <t>00:05</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr">
+      <c r="H64" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
@@ -2764,15 +3084,20 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
           <t>01:28</t>
         </is>
       </c>
-      <c r="G65" t="inlineStr">
+      <c r="H65" t="inlineStr">
         <is>
           <t>08:28</t>
         </is>
@@ -2791,27 +3116,74 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:21 | 12:00 | 13:00 | 16:21</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
           <t>08:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>14/01/2026</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>08:00 | 11:34 | 12:34 | 16:05</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>07:05</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>-00:55</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>07:33</t>
         </is>
       </c>
     </row>

</xml_diff>